<commit_message>
scoring program and scoring excel
</commit_message>
<xml_diff>
--- a/Sampledata_Comet_Allcolumns_updated28thAug.xlsx
+++ b/Sampledata_Comet_Allcolumns_updated28thAug.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\azfarjef\42KL\DHL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1D46D1-1CB5-4F3D-B5EC-A3B87B45E44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C3BCDB-0555-4FA9-8F66-68C78CE3B0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25798" yWindow="1943" windowWidth="14671" windowHeight="13924" activeTab="2" xr2:uid="{42CE140A-3AB5-438F-8412-76FAA93178C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{42CE140A-3AB5-438F-8412-76FAA93178C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Column heads and explanation" sheetId="3" r:id="rId1"/>
     <sheet name="Sample Records " sheetId="4" r:id="rId2"/>
-    <sheet name="test" sheetId="5" r:id="rId3"/>
+    <sheet name="data_structure" sheetId="6" r:id="rId3"/>
+    <sheet name="scoring" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="213">
   <si>
     <t>KUALA LUMPUR</t>
   </si>
@@ -384,107 +387,302 @@
     <t xml:space="preserve">Kindly feel free to add / recommend columns which can be useful for lead scoring/ lead prioritization . Lead status column can alos be inlcuded to map what the current stage of the lead within DHL </t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>ahmad</t>
-  </si>
-  <si>
-    <t>ali</t>
-  </si>
-  <si>
-    <t>abu</t>
-  </si>
-  <si>
-    <t>ah chong</t>
-  </si>
-  <si>
-    <t>raju</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Contact no</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>a.com</t>
-  </si>
-  <si>
-    <t>b.com</t>
-  </si>
-  <si>
-    <t>c.com</t>
-  </si>
-  <si>
-    <t>d.com</t>
-  </si>
-  <si>
-    <t>e.com</t>
-  </si>
-  <si>
-    <t>siti</t>
-  </si>
-  <si>
-    <t>asfs</t>
-  </si>
-  <si>
-    <t>fs</t>
-  </si>
-  <si>
-    <t>sf</t>
-  </si>
-  <si>
-    <t>sfds</t>
-  </si>
-  <si>
-    <t>sdgsdg</t>
-  </si>
-  <si>
-    <t>dgfdh</t>
-  </si>
-  <si>
-    <t>hdfgdf</t>
-  </si>
-  <si>
-    <t>hfhd</t>
-  </si>
-  <si>
-    <t>fdh</t>
-  </si>
-  <si>
-    <t>HAHAHA</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>f.com</t>
+    <t>Company Details</t>
+  </si>
+  <si>
+    <t>Unique_id</t>
+  </si>
+  <si>
+    <t>Company_name</t>
+  </si>
+  <si>
+    <t>Company_address</t>
+  </si>
+  <si>
+    <t>Employee_count</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Main_phone_number</t>
+  </si>
+  <si>
+    <t>Physical_channel</t>
+  </si>
+  <si>
+    <t>SSM_number</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Total_potential_revenue/month</t>
+  </si>
+  <si>
+    <t>Contact Details</t>
+  </si>
+  <si>
+    <t>Contact_name</t>
+  </si>
+  <si>
+    <t>Contact_email</t>
+  </si>
+  <si>
+    <t>Contact_no</t>
+  </si>
+  <si>
+    <t>Contact_Designation</t>
+  </si>
+  <si>
+    <t>Lead Generation</t>
+  </si>
+  <si>
+    <t>Lead_source_name</t>
+  </si>
+  <si>
+    <t>Lead_source_details</t>
+  </si>
+  <si>
+    <t>Suspect_creation_date</t>
+  </si>
+  <si>
+    <t>Suspect_creation_by</t>
+  </si>
+  <si>
+    <t>Suspect_accepted_by</t>
+  </si>
+  <si>
+    <t>Suspect_accepted_at</t>
+  </si>
+  <si>
+    <t>Prospect_accepted_by</t>
+  </si>
+  <si>
+    <t>Prospect_accepted_at</t>
+  </si>
+  <si>
+    <t>Lead_score</t>
+  </si>
+  <si>
+    <t>Lead_margin</t>
+  </si>
+  <si>
+    <t>Existing_customer</t>
+  </si>
+  <si>
+    <t>Contact_linkedin</t>
+  </si>
+  <si>
+    <t>Extra Column</t>
+  </si>
+  <si>
+    <t>Company establish date</t>
+  </si>
+  <si>
+    <t>Weightage</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Service logistics</t>
+  </si>
+  <si>
+    <t>Life Sciences and Healthcare</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Chemical and Energy</t>
+  </si>
+  <si>
+    <t>Distributor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service  </t>
+  </si>
+  <si>
+    <t>Suspect creation date</t>
+  </si>
+  <si>
+    <t>&gt; 6 months</t>
+  </si>
+  <si>
+    <t>&gt; 12 months</t>
+  </si>
+  <si>
+    <t>3-6 months</t>
+  </si>
+  <si>
+    <t>&lt; 3 months</t>
+  </si>
+  <si>
+    <t>Prospect accepted</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Null/Not accepted</t>
+  </si>
+  <si>
+    <t>Prospect creation date</t>
+  </si>
+  <si>
+    <t>&gt; 3 months</t>
+  </si>
+  <si>
+    <t>&gt; 1 months</t>
+  </si>
+  <si>
+    <t>1 months</t>
+  </si>
+  <si>
+    <t>&lt; 10 days</t>
+  </si>
+  <si>
+    <t>Employee count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 100 </t>
+  </si>
+  <si>
+    <t>50 - 100</t>
+  </si>
+  <si>
+    <t>1 till 50</t>
+  </si>
+  <si>
+    <t>Total potential revenue</t>
+  </si>
+  <si>
+    <t>&gt; 1000</t>
+  </si>
+  <si>
+    <t>500 - 1000</t>
+  </si>
+  <si>
+    <t>100 - 500</t>
+  </si>
+  <si>
+    <t>&lt; 100</t>
+  </si>
+  <si>
+    <t>Non-profit</t>
+  </si>
+  <si>
+    <t>Competitor</t>
+  </si>
+  <si>
+    <t>Competitors company</t>
+  </si>
+  <si>
+    <t>Already have courier partner</t>
+  </si>
+  <si>
+    <t>Don’t have</t>
+  </si>
+  <si>
+    <t>Contact information</t>
+  </si>
+  <si>
+    <t>Lead source</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>ex database</t>
+  </si>
+  <si>
+    <t>content blogs</t>
+  </si>
+  <si>
+    <t>signup pages</t>
+  </si>
+  <si>
+    <t>exhibitions</t>
+  </si>
+  <si>
+    <t>procured from market</t>
+  </si>
+  <si>
+    <t>All Null</t>
+  </si>
+  <si>
+    <t>Null phone no.</t>
+  </si>
+  <si>
+    <t>Null email</t>
+  </si>
+  <si>
+    <t>Have both</t>
+  </si>
+  <si>
+    <t>Lead margin</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>Warm</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>70-100</t>
+  </si>
+  <si>
+    <t>40-69</t>
+  </si>
+  <si>
+    <t>0-39</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>&lt; 0</t>
+  </si>
+  <si>
+    <t>Final Ranking</t>
+  </si>
+  <si>
+    <t>Company name</t>
+  </si>
+  <si>
+    <t>Employee Count</t>
+  </si>
+  <si>
+    <t>Last Created</t>
+  </si>
+  <si>
+    <t>Existing Customer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,8 +733,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,6 +763,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,7 +812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -619,8 +830,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -938,18 +1157,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7994818C-0006-4C4F-AF36-45EDB5458467}">
   <dimension ref="B2:D35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="63.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.25" customWidth="1"/>
-    <col min="4" max="4" width="178.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
+    <col min="4" max="4" width="178.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="15" t="s">
         <v>49</v>
       </c>
@@ -960,7 +1179,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>54</v>
       </c>
@@ -971,7 +1190,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -982,7 +1201,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>35</v>
       </c>
@@ -993,7 +1212,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>41</v>
       </c>
@@ -1004,7 +1223,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>69</v>
       </c>
@@ -1015,43 +1234,43 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" s="5" t="s">
         <v>43</v>
       </c>
@@ -1059,27 +1278,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C17" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C18" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>33</v>
       </c>
@@ -1090,7 +1309,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>40</v>
       </c>
@@ -1098,7 +1317,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
         <v>13</v>
       </c>
@@ -1106,7 +1325,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1114,7 +1333,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
         <v>87</v>
       </c>
@@ -1122,7 +1341,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>51</v>
       </c>
@@ -1133,7 +1352,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>50</v>
       </c>
@@ -1141,7 +1360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>52</v>
       </c>
@@ -1152,7 +1371,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>48</v>
       </c>
@@ -1160,7 +1379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
@@ -1171,7 +1390,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>37</v>
       </c>
@@ -1182,17 +1401,17 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>114</v>
       </c>
@@ -1204,40 +1423,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF12ABA-7989-4BAA-ADAA-80919704EBB2}">
-  <dimension ref="A1:AC15"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView showGridLines="0" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="36.125" customWidth="1"/>
-    <col min="4" max="4" width="35.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="12.125" customWidth="1"/>
-    <col min="16" max="16" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12.109375" customWidth="1"/>
+    <col min="16" max="16" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="38" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="38" customWidth="1"/>
-    <col min="21" max="21" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.625" customWidth="1"/>
-    <col min="26" max="26" width="20.125" customWidth="1"/>
-    <col min="27" max="27" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.6640625" customWidth="1"/>
+    <col min="26" max="26" width="20.109375" customWidth="1"/>
+    <col min="27" max="27" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.625" customWidth="1"/>
+    <col min="29" max="29" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>38</v>
       </c>
@@ -1324,7 +1543,7 @@
       </c>
       <c r="AC1" s="16"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>68</v>
       </c>
@@ -1372,7 +1591,7 @@
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1420,7 +1639,7 @@
       <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1466,7 +1685,7 @@
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1510,7 +1729,7 @@
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1554,7 +1773,7 @@
       <c r="AA6" s="7"/>
       <c r="AB6" s="7"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1596,7 +1815,7 @@
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1640,7 +1859,7 @@
       <c r="AA8" s="7"/>
       <c r="AB8" s="7"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1684,7 +1903,7 @@
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1728,7 +1947,7 @@
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1771,60 +1990,6 @@
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F12" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F13" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F14" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="L14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F15" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q15" s="18" t="s">
-        <v>75</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1836,178 +2001,695 @@
     <hyperlink ref="R6" r:id="rId5" display="B@B" xr:uid="{12BF1425-D14E-40D5-ADBF-FAC60308839D}"/>
     <hyperlink ref="R8" r:id="rId6" display="B@B" xr:uid="{000960CE-26A5-42AA-8588-69FE8A99EFCA}"/>
     <hyperlink ref="R10" r:id="rId7" display="B@B" xr:uid="{A0A7CB35-C530-4BF9-AFBB-D2E5D0C407C7}"/>
-    <hyperlink ref="Q15" r:id="rId8" xr:uid="{398EBFFD-1332-411A-AF6C-5C34513A5AEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC4BA38-D919-4064-9520-1EDAC4BC8728}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E55C22C-9752-47E5-AE6F-01ED0706CBAB}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A13:F13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2036BEE-BD0C-464F-8838-1BDB0167799B}">
+  <dimension ref="A1:S29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" t="s">
-        <v>129</v>
+        <v>147</v>
+      </c>
+      <c r="C1">
+        <v>0.3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1">
+        <v>0.15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="17">
-        <v>60123456789</v>
-      </c>
-      <c r="D2" t="s">
-        <v>116</v>
+      <c r="M1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O1">
+        <v>0.2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>172</v>
+      </c>
+      <c r="R1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>119</v>
+        <v>160</v>
+      </c>
+      <c r="G2">
+        <v>-50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O2">
+        <v>-100</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>173</v>
+      </c>
+      <c r="S2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>149</v>
       </c>
       <c r="C3">
-        <v>60323549858</v>
-      </c>
-      <c r="D3" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>120</v>
+        <v>161</v>
+      </c>
+      <c r="G3">
+        <v>-100</v>
+      </c>
+      <c r="I3" t="s">
+        <v>166</v>
+      </c>
+      <c r="K3">
+        <v>-50</v>
+      </c>
+      <c r="M3" t="s">
+        <v>169</v>
+      </c>
+      <c r="O3">
+        <v>-50</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>174</v>
+      </c>
+      <c r="S3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>148</v>
       </c>
       <c r="C4">
-        <v>60122314553</v>
-      </c>
-      <c r="D4" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>121</v>
+        <v>162</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="M4" t="s">
+        <v>170</v>
+      </c>
+      <c r="O4">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="S4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>151</v>
       </c>
       <c r="C5">
-        <v>60472732843</v>
-      </c>
-      <c r="D5" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
+        <v>163</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="M5" t="s">
+        <v>171</v>
+      </c>
+      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>155</v>
       </c>
       <c r="C6">
-        <v>60324238858</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>122</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>157</v>
       </c>
       <c r="C11">
-        <v>60324238858</v>
-      </c>
-      <c r="E11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" t="s">
         <v>147</v>
+      </c>
+      <c r="C15">
+        <v>0.1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15">
+        <v>0.5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>182</v>
+      </c>
+      <c r="J15" t="s">
+        <v>147</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>186</v>
+      </c>
+      <c r="N15" t="s">
+        <v>147</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>187</v>
+      </c>
+      <c r="R15" t="s">
+        <v>147</v>
+      </c>
+      <c r="S15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="I16" t="s">
+        <v>183</v>
+      </c>
+      <c r="K16">
+        <v>-100</v>
+      </c>
+      <c r="M16" t="s">
+        <v>195</v>
+      </c>
+      <c r="O16">
+        <v>-20</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>188</v>
+      </c>
+      <c r="S16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17">
+        <v>80</v>
+      </c>
+      <c r="I17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K17">
+        <v>-100</v>
+      </c>
+      <c r="M17" t="s">
+        <v>197</v>
+      </c>
+      <c r="O17">
+        <v>-15</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>189</v>
+      </c>
+      <c r="S17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G18">
+        <v>-50</v>
+      </c>
+      <c r="I18" t="s">
+        <v>185</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>196</v>
+      </c>
+      <c r="O18">
+        <v>-10</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>190</v>
+      </c>
+      <c r="S18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="M19" t="s">
+        <v>198</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>191</v>
+      </c>
+      <c r="S19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q20" t="s">
+        <v>192</v>
+      </c>
+      <c r="S20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q21" t="s">
+        <v>193</v>
+      </c>
+      <c r="S21">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q22" t="s">
+        <v>194</v>
+      </c>
+      <c r="S22">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>206</v>
+      </c>
+      <c r="B29" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify unique_gen and weightedscore program
</commit_message>
<xml_diff>
--- a/Sampledata_Comet_Allcolumns_updated28thAug.xlsx
+++ b/Sampledata_Comet_Allcolumns_updated28thAug.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C3BCDB-0555-4FA9-8F66-68C78CE3B0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843DB387-733E-4236-958C-CC51B7BB6966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{42CE140A-3AB5-438F-8412-76FAA93178C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{42CE140A-3AB5-438F-8412-76FAA93178C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Column heads and explanation" sheetId="3" r:id="rId1"/>
@@ -2010,8 +2010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E55C22C-9752-47E5-AE6F-01ED0706CBAB}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2243,7 +2243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2036BEE-BD0C-464F-8838-1BDB0167799B}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>